<commit_message>
[ADD] Action Plan + Summary
</commit_message>
<xml_diff>
--- a/Team Docs/PeerReview.xlsx
+++ b/Team Docs/PeerReview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Y2\Block 3\Project startup\Design Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project-startup\Team Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF94A26-3B4C-481D-8877-753F04811E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9F159F-2174-4B8E-97D0-DBA299886A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10308" yWindow="3648" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 2 Review" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,18 @@
     <sheet name="Progress Overview" sheetId="4" r:id="rId4"/>
     <sheet name="Data" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -308,14 +312,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Strength(s): Madre the initial prototyoe very quicjly
-and never says no to adding a new feature, adds 
-logiical feedback when talking about dsign
-Improvement(s): Sometimes get stuck onj points
-during discussions
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Strength(s): Reacting well to being lead of other programmers, knowledge of engine programming 
 helping the project along, good communication
 Improvement(s): At times gets stuck on tiny details when
@@ -404,6 +400,14 @@
 You deliver your work in a timely manner to the best of your abilities. Despite having daunting complicated tasks in an unknown engine and with a failry daunting unknown language you don't shy away from struggling through it anyways and delivering performance.
 Improvement(s):
 C++ skills in more advanced topics could be improved. You lack confidence in your code. You are a good programmer, acknowledge that.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s): Made the initial prototype very quicky
+and never says no to adding a new feature, adds 
+logical feedback when talking about design
+Improvement(s): Sometimes get stuck on points
+during discussions
+</t>
   </si>
 </sst>
 </file>
@@ -784,6 +788,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -815,7 +820,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,6 +1286,58 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1585,8 +1641,8 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="J4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1626,33 +1682,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="55" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1662,31 +1718,31 @@
         <v>12</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
     </row>
     <row r="3" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1698,31 +1754,31 @@
       <c r="C3" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="57"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
@@ -1790,28 +1846,28 @@
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="16" t="s">
         <v>20</v>
@@ -1904,8 +1960,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="63" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+    <row r="7" spans="1:26" s="46" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="62" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="20">
@@ -1933,19 +1989,19 @@
         <v>8</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="K7" s="42">
         <v>8</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M7" s="24">
         <v>8</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O7" s="24">
         <v>7</v>
@@ -1971,7 +2027,7 @@
       <c r="Z7" s="45"/>
     </row>
     <row r="8" spans="1:26" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="20">
         <v>464704</v>
       </c>
@@ -2034,8 +2090,8 @@
       <c r="Y8" s="26"/>
       <c r="Z8" s="27"/>
     </row>
-    <row r="9" spans="1:26" s="63" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+    <row r="9" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
       <c r="B9" s="20">
         <v>428729</v>
       </c>
@@ -2043,37 +2099,37 @@
         <v>51</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="42">
         <v>10</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G9" s="42">
         <v>10</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I9" s="42">
         <v>7</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K9" s="42">
         <v>10</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M9" s="24">
         <v>10</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O9" s="24">
         <v>10</v>
@@ -2098,8 +2154,8 @@
       <c r="Y9" s="26"/>
       <c r="Z9" s="27"/>
     </row>
-    <row r="10" spans="1:26" s="63" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+    <row r="10" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
       <c r="B10" s="20">
         <v>444711</v>
       </c>
@@ -2162,8 +2218,8 @@
       <c r="Y10" s="26"/>
       <c r="Z10" s="27"/>
     </row>
-    <row r="11" spans="1:26" s="63" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+    <row r="11" spans="1:26" s="46" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
       <c r="B11" s="20">
         <v>445021</v>
       </c>
@@ -2171,37 +2227,37 @@
         <v>47</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="24">
         <v>8</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" s="24">
         <v>8</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I11" s="24">
         <v>8</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K11" s="24">
         <v>8</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M11" s="24">
         <v>7</v>
       </c>
       <c r="N11" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O11" s="24">
         <v>8</v>
@@ -2227,7 +2283,7 @@
       <c r="Z11" s="27"/>
     </row>
     <row r="12" spans="1:26" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="20">
         <v>459575</v>
       </c>
@@ -2279,7 +2335,7 @@
       <c r="Z12" s="27"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="20">
         <v>12335</v>
       </c>
@@ -2331,7 +2387,7 @@
       <c r="Z13" s="27"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="20">
         <v>12335</v>
       </c>
@@ -2383,7 +2439,7 @@
       <c r="Z14" s="27"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="20">
         <v>12335</v>
       </c>
@@ -2435,7 +2491,7 @@
       <c r="Z15" s="27"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="20">
         <v>12335</v>
       </c>
@@ -2565,34 +2621,34 @@
       <c r="Z17" s="32"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="59"/>
-      <c r="X18" s="59"/>
-      <c r="Y18" s="59"/>
-      <c r="Z18" s="60"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="60"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2651,186 +2707,186 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="46" priority="26" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="45" priority="27" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="44" priority="28" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="29" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="30" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="31" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="18" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="19" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="20" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="21" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="22" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="17" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="23" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="14" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2922,33 +2978,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="55" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2956,31 +3012,31 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2990,31 +3046,31 @@
         <v>7</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="57"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
@@ -3082,28 +3138,28 @@
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="16" t="s">
         <v>20</v>
@@ -3197,7 +3253,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="62" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="20">
@@ -3251,7 +3307,7 @@
       <c r="Z7" s="27"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="20">
         <v>12335</v>
       </c>
@@ -3303,7 +3359,7 @@
       <c r="Z8" s="27"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="20">
         <v>12335</v>
       </c>
@@ -3355,7 +3411,7 @@
       <c r="Z9" s="27"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="20">
         <v>12335</v>
       </c>
@@ -3407,7 +3463,7 @@
       <c r="Z10" s="27"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="20">
         <v>12335</v>
       </c>
@@ -3459,7 +3515,7 @@
       <c r="Z11" s="27"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="20">
         <v>12335</v>
       </c>
@@ -3511,7 +3567,7 @@
       <c r="Z12" s="27"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="20">
         <v>12335</v>
       </c>
@@ -3563,7 +3619,7 @@
       <c r="Z13" s="27"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="20">
         <v>12335</v>
       </c>
@@ -3615,7 +3671,7 @@
       <c r="Z14" s="27"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="20">
         <v>12335</v>
       </c>
@@ -3667,7 +3723,7 @@
       <c r="Z15" s="27"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="20">
         <v>12335</v>
       </c>
@@ -3797,34 +3853,34 @@
       <c r="Z17" s="32"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="59"/>
-      <c r="X18" s="59"/>
-      <c r="Y18" s="59"/>
-      <c r="Z18" s="60"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="60"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3837,48 +3893,48 @@
     <mergeCell ref="D5:W5"/>
   </mergeCells>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="41" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="40" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3946,33 +4002,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="55" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3980,31 +4036,31 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4014,31 +4070,31 @@
         <v>7</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="57"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
@@ -4106,28 +4162,28 @@
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="16" t="s">
         <v>20</v>
@@ -4221,7 +4277,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="62" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="20">
@@ -4275,7 +4331,7 @@
       <c r="Z7" s="27"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="20">
         <v>12335</v>
       </c>
@@ -4327,7 +4383,7 @@
       <c r="Z8" s="27"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="20">
         <v>12335</v>
       </c>
@@ -4379,7 +4435,7 @@
       <c r="Z9" s="27"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="20">
         <v>12335</v>
       </c>
@@ -4431,7 +4487,7 @@
       <c r="Z10" s="27"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="20">
         <v>12335</v>
       </c>
@@ -4483,7 +4539,7 @@
       <c r="Z11" s="27"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="20">
         <v>12335</v>
       </c>
@@ -4535,7 +4591,7 @@
       <c r="Z12" s="27"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="20">
         <v>12335</v>
       </c>
@@ -4587,7 +4643,7 @@
       <c r="Z13" s="27"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="20">
         <v>12335</v>
       </c>
@@ -4639,7 +4695,7 @@
       <c r="Z14" s="27"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="20">
         <v>12335</v>
       </c>
@@ -4691,7 +4747,7 @@
       <c r="Z15" s="27"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="20">
         <v>12335</v>
       </c>
@@ -4821,34 +4877,34 @@
       <c r="Z17" s="32"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="59"/>
-      <c r="X18" s="59"/>
-      <c r="Y18" s="59"/>
-      <c r="Z18" s="60"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="60"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4861,48 +4917,48 @@
     <mergeCell ref="D5:W5"/>
   </mergeCells>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>